<commit_message>
outputs mapping updated with chemicals link
</commit_message>
<xml_diff>
--- a/knowledge-graph/mappings/outputs-solarchem-mapping.xlsx
+++ b/knowledge-graph/mappings/outputs-solarchem-mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/GitHub/solarchem-ontology/knowledge-graph/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E62AAA7-1960-0546-876C-ADFEEE844763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1288F019-08B2-0C4C-8F32-CCF9E3A3C848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefix" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1323" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1527" uniqueCount="249">
   <si>
     <t>Prefix</t>
   </si>
@@ -730,6 +730,60 @@
   </si>
   <si>
     <t>http://qudt.org/2.1/schema/qudt/</t>
+  </si>
+  <si>
+    <t>solar:hasChemical</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q3027893</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q2025</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q37129</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q151313</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q52858</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q151324</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q131189</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q151335</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q134192</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q151353</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q2799651</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q14982</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q153</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q61457</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q161233</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q161210</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q47512</t>
   </si>
 </sst>
 </file>
@@ -1139,7 +1193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -2518,8 +2572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="A36" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A18" sqref="A2:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3134,17 +3188,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H213"/>
+  <dimension ref="A1:H266"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A161" sqref="A161:A213"/>
+    <sheetView tabSelected="1" topLeftCell="A204" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E219" sqref="E219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" customWidth="1"/>
-    <col min="3" max="3" width="33.6640625" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
     <col min="6" max="6" width="12.5" customWidth="1"/>
@@ -6094,6 +6148,729 @@
       <c r="D213" t="s">
         <v>42</v>
       </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A214" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B214" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C214" t="s">
+        <v>232</v>
+      </c>
+      <c r="D214" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A215" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B215" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C215" t="s">
+        <v>233</v>
+      </c>
+      <c r="D215" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A216" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B216" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C216" t="s">
+        <v>234</v>
+      </c>
+      <c r="D216" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A217" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B217" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C217" t="s">
+        <v>235</v>
+      </c>
+      <c r="D217" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A218" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B218" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C218" t="s">
+        <v>236</v>
+      </c>
+      <c r="D218" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A219" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B219" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C219" t="s">
+        <v>237</v>
+      </c>
+      <c r="D219" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A220" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B220" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C220" t="s">
+        <v>238</v>
+      </c>
+      <c r="D220" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A221" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B221" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C221" t="s">
+        <v>239</v>
+      </c>
+      <c r="D221" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A222" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B222" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C222" t="s">
+        <v>240</v>
+      </c>
+      <c r="D222" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A223" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B223" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C223" t="s">
+        <v>241</v>
+      </c>
+      <c r="D223" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A224" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B224" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C224" t="s">
+        <v>242</v>
+      </c>
+      <c r="D224" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A225" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B225" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C225" t="s">
+        <v>243</v>
+      </c>
+      <c r="D225" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A226" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B226" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C226" t="s">
+        <v>244</v>
+      </c>
+      <c r="D226" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A227" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B227" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C227" t="s">
+        <v>245</v>
+      </c>
+      <c r="D227" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A228" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B228" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C228" t="s">
+        <v>246</v>
+      </c>
+      <c r="D228" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A229" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B229" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C229" t="s">
+        <v>247</v>
+      </c>
+      <c r="D229" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A230" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B230" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C230" t="s">
+        <v>248</v>
+      </c>
+      <c r="D230" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A231" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B231" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C231" t="s">
+        <v>232</v>
+      </c>
+      <c r="D231" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A232" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B232" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C232" t="s">
+        <v>233</v>
+      </c>
+      <c r="D232" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A233" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B233" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C233" t="s">
+        <v>234</v>
+      </c>
+      <c r="D233" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A234" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B234" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C234" t="s">
+        <v>235</v>
+      </c>
+      <c r="D234" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A235" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B235" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C235" t="s">
+        <v>236</v>
+      </c>
+      <c r="D235" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A236" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B236" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C236" t="s">
+        <v>237</v>
+      </c>
+      <c r="D236" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A237" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B237" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C237" t="s">
+        <v>238</v>
+      </c>
+      <c r="D237" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A238" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B238" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C238" t="s">
+        <v>239</v>
+      </c>
+      <c r="D238" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A239" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B239" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C239" t="s">
+        <v>240</v>
+      </c>
+      <c r="D239" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A240" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B240" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C240" t="s">
+        <v>241</v>
+      </c>
+      <c r="D240" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A241" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B241" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C241" t="s">
+        <v>242</v>
+      </c>
+      <c r="D241" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A242" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B242" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C242" t="s">
+        <v>243</v>
+      </c>
+      <c r="D242" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A243" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B243" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C243" t="s">
+        <v>244</v>
+      </c>
+      <c r="D243" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A244" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B244" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C244" t="s">
+        <v>245</v>
+      </c>
+      <c r="D244" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A245" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B245" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C245" t="s">
+        <v>246</v>
+      </c>
+      <c r="D245" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A246" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B246" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C246" t="s">
+        <v>247</v>
+      </c>
+      <c r="D246" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A247" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B247" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C247" t="s">
+        <v>248</v>
+      </c>
+      <c r="D247" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A248" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B248" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C248" t="s">
+        <v>232</v>
+      </c>
+      <c r="D248" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A249" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B249" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C249" t="s">
+        <v>233</v>
+      </c>
+      <c r="D249" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A250" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B250" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C250" t="s">
+        <v>234</v>
+      </c>
+      <c r="D250" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A251" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B251" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C251" t="s">
+        <v>235</v>
+      </c>
+      <c r="D251" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A252" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B252" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C252" t="s">
+        <v>236</v>
+      </c>
+      <c r="D252" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A253" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B253" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C253" t="s">
+        <v>237</v>
+      </c>
+      <c r="D253" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A254" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B254" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C254" t="s">
+        <v>238</v>
+      </c>
+      <c r="D254" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A255" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B255" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C255" t="s">
+        <v>239</v>
+      </c>
+      <c r="D255" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A256" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B256" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C256" t="s">
+        <v>240</v>
+      </c>
+      <c r="D256" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A257" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B257" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C257" t="s">
+        <v>241</v>
+      </c>
+      <c r="D257" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A258" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B258" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C258" t="s">
+        <v>242</v>
+      </c>
+      <c r="D258" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A259" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B259" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C259" t="s">
+        <v>243</v>
+      </c>
+      <c r="D259" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A260" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B260" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C260" t="s">
+        <v>244</v>
+      </c>
+      <c r="D260" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A261" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B261" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C261" t="s">
+        <v>245</v>
+      </c>
+      <c r="D261" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A262" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B262" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C262" t="s">
+        <v>246</v>
+      </c>
+      <c r="D262" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A263" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B263" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C263" t="s">
+        <v>247</v>
+      </c>
+      <c r="D263" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A264" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B264" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C264" t="s">
+        <v>248</v>
+      </c>
+      <c r="D264" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A265" s="10"/>
+      <c r="B265" s="7"/>
+      <c r="D265" s="10"/>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A266" s="10"/>
+      <c r="B266" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
selectivity added in onto, diagrams, doc and mappings
</commit_message>
<xml_diff>
--- a/knowledge-graph/mappings/outputs-solarchem-mapping.xlsx
+++ b/knowledge-graph/mappings/outputs-solarchem-mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/GitHub/solarchem-ontology/knowledge-graph/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDC0D02-B802-DA49-86A7-E9623A3FE359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0EEF08-CCAB-944E-929E-81A8308F6C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="28800" windowHeight="17500" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="267">
   <si>
     <t>Prefix</t>
   </si>
@@ -823,6 +823,21 @@
   </si>
   <si>
     <t>http://www.wikidata.org/entity/Q1999</t>
+  </si>
+  <si>
+    <t>solar:selectivityPercentage</t>
+  </si>
+  <si>
+    <t>{h2_selectivity_molg}</t>
+  </si>
+  <si>
+    <t>{co_selectivity_molg}</t>
+  </si>
+  <si>
+    <t>{ch4_selectivity_molg}</t>
+  </si>
+  <si>
+    <t>{ch3oh_selectivity_molg}</t>
   </si>
 </sst>
 </file>
@@ -901,7 +916,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -915,7 +930,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -935,9 +949,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -975,7 +989,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1081,7 +1095,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1223,7 +1237,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3292,7 +3306,7 @@
       <c r="B55" t="s">
         <v>172</v>
       </c>
-      <c r="C55" s="11" t="s">
+      <c r="C55" t="s">
         <v>252</v>
       </c>
     </row>
@@ -3303,7 +3317,7 @@
       <c r="B56" t="s">
         <v>172</v>
       </c>
-      <c r="C56" s="11" t="s">
+      <c r="C56" t="s">
         <v>253</v>
       </c>
     </row>
@@ -3314,7 +3328,7 @@
       <c r="B57" t="s">
         <v>172</v>
       </c>
-      <c r="C57" s="11" t="s">
+      <c r="C57" t="s">
         <v>254</v>
       </c>
     </row>
@@ -3327,16 +3341,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H279"/>
+  <dimension ref="A1:H283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A255" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C213" sqref="C161:C213"/>
+    <sheetView tabSelected="1" topLeftCell="A261" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C284" sqref="C284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
     <col min="3" max="3" width="37.33203125" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
@@ -5553,7 +5567,7 @@
       <c r="B161" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C161" s="11" t="s">
+      <c r="C161" t="s">
         <v>248</v>
       </c>
       <c r="D161" t="s">
@@ -5567,7 +5581,7 @@
       <c r="B162" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C162" s="11" t="s">
+      <c r="C162" t="s">
         <v>248</v>
       </c>
       <c r="D162" t="s">
@@ -5581,7 +5595,7 @@
       <c r="B163" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C163" s="11" t="s">
+      <c r="C163" t="s">
         <v>248</v>
       </c>
       <c r="D163" t="s">
@@ -5595,7 +5609,7 @@
       <c r="B164" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C164" s="11" t="s">
+      <c r="C164" t="s">
         <v>248</v>
       </c>
       <c r="D164" t="s">
@@ -5609,7 +5623,7 @@
       <c r="B165" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C165" s="11" t="s">
+      <c r="C165" t="s">
         <v>248</v>
       </c>
       <c r="D165" t="s">
@@ -5623,7 +5637,7 @@
       <c r="B166" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C166" s="11" t="s">
+      <c r="C166" t="s">
         <v>248</v>
       </c>
       <c r="D166" t="s">
@@ -5637,7 +5651,7 @@
       <c r="B167" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C167" s="11" t="s">
+      <c r="C167" t="s">
         <v>248</v>
       </c>
       <c r="D167" t="s">
@@ -5651,7 +5665,7 @@
       <c r="B168" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C168" s="11" t="s">
+      <c r="C168" t="s">
         <v>248</v>
       </c>
       <c r="D168" t="s">
@@ -5665,7 +5679,7 @@
       <c r="B169" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C169" s="11" t="s">
+      <c r="C169" t="s">
         <v>248</v>
       </c>
       <c r="D169" t="s">
@@ -5679,7 +5693,7 @@
       <c r="B170" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C170" s="11" t="s">
+      <c r="C170" t="s">
         <v>248</v>
       </c>
       <c r="D170" t="s">
@@ -5693,7 +5707,7 @@
       <c r="B171" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C171" s="11" t="s">
+      <c r="C171" t="s">
         <v>248</v>
       </c>
       <c r="D171" t="s">
@@ -5707,7 +5721,7 @@
       <c r="B172" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C172" s="11" t="s">
+      <c r="C172" t="s">
         <v>248</v>
       </c>
       <c r="D172" t="s">
@@ -5721,7 +5735,7 @@
       <c r="B173" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C173" s="11" t="s">
+      <c r="C173" t="s">
         <v>248</v>
       </c>
       <c r="D173" t="s">
@@ -5735,7 +5749,7 @@
       <c r="B174" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C174" s="11" t="s">
+      <c r="C174" t="s">
         <v>248</v>
       </c>
       <c r="D174" t="s">
@@ -5749,7 +5763,7 @@
       <c r="B175" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C175" s="11" t="s">
+      <c r="C175" t="s">
         <v>248</v>
       </c>
       <c r="D175" t="s">
@@ -5763,7 +5777,7 @@
       <c r="B176" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C176" s="11" t="s">
+      <c r="C176" t="s">
         <v>248</v>
       </c>
       <c r="D176" t="s">
@@ -5777,7 +5791,7 @@
       <c r="B177" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C177" s="11" t="s">
+      <c r="C177" t="s">
         <v>248</v>
       </c>
       <c r="D177" t="s">
@@ -5791,7 +5805,7 @@
       <c r="B178" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C178" s="11" t="s">
+      <c r="C178" t="s">
         <v>248</v>
       </c>
       <c r="D178" t="s">
@@ -5805,7 +5819,7 @@
       <c r="B179" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C179" s="11" t="s">
+      <c r="C179" t="s">
         <v>248</v>
       </c>
       <c r="D179" t="s">
@@ -5819,7 +5833,7 @@
       <c r="B180" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C180" s="11" t="s">
+      <c r="C180" t="s">
         <v>248</v>
       </c>
       <c r="D180" t="s">
@@ -5833,7 +5847,7 @@
       <c r="B181" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C181" s="11" t="s">
+      <c r="C181" t="s">
         <v>248</v>
       </c>
       <c r="D181" t="s">
@@ -5847,7 +5861,7 @@
       <c r="B182" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C182" s="11" t="s">
+      <c r="C182" t="s">
         <v>248</v>
       </c>
       <c r="D182" t="s">
@@ -5861,7 +5875,7 @@
       <c r="B183" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C183" s="11" t="s">
+      <c r="C183" t="s">
         <v>248</v>
       </c>
       <c r="D183" t="s">
@@ -5875,7 +5889,7 @@
       <c r="B184" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C184" s="11" t="s">
+      <c r="C184" t="s">
         <v>248</v>
       </c>
       <c r="D184" t="s">
@@ -5889,7 +5903,7 @@
       <c r="B185" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C185" s="11" t="s">
+      <c r="C185" t="s">
         <v>248</v>
       </c>
       <c r="D185" t="s">
@@ -5903,7 +5917,7 @@
       <c r="B186" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C186" s="11" t="s">
+      <c r="C186" t="s">
         <v>248</v>
       </c>
       <c r="D186" t="s">
@@ -5917,7 +5931,7 @@
       <c r="B187" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C187" s="11" t="s">
+      <c r="C187" t="s">
         <v>248</v>
       </c>
       <c r="D187" t="s">
@@ -5931,7 +5945,7 @@
       <c r="B188" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C188" s="11" t="s">
+      <c r="C188" t="s">
         <v>248</v>
       </c>
       <c r="D188" t="s">
@@ -5945,7 +5959,7 @@
       <c r="B189" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C189" s="11" t="s">
+      <c r="C189" t="s">
         <v>248</v>
       </c>
       <c r="D189" t="s">
@@ -5959,7 +5973,7 @@
       <c r="B190" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C190" s="11" t="s">
+      <c r="C190" t="s">
         <v>248</v>
       </c>
       <c r="D190" t="s">
@@ -5973,7 +5987,7 @@
       <c r="B191" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C191" s="11" t="s">
+      <c r="C191" t="s">
         <v>248</v>
       </c>
       <c r="D191" t="s">
@@ -5987,7 +6001,7 @@
       <c r="B192" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C192" s="11" t="s">
+      <c r="C192" t="s">
         <v>248</v>
       </c>
       <c r="D192" t="s">
@@ -6001,7 +6015,7 @@
       <c r="B193" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C193" s="11" t="s">
+      <c r="C193" t="s">
         <v>248</v>
       </c>
       <c r="D193" t="s">
@@ -6015,7 +6029,7 @@
       <c r="B194" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C194" s="11" t="s">
+      <c r="C194" t="s">
         <v>248</v>
       </c>
       <c r="D194" t="s">
@@ -6029,7 +6043,7 @@
       <c r="B195" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C195" s="11" t="s">
+      <c r="C195" t="s">
         <v>248</v>
       </c>
       <c r="D195" t="s">
@@ -6043,7 +6057,7 @@
       <c r="B196" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C196" s="11" t="s">
+      <c r="C196" t="s">
         <v>248</v>
       </c>
       <c r="D196" t="s">
@@ -6057,7 +6071,7 @@
       <c r="B197" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C197" s="11" t="s">
+      <c r="C197" t="s">
         <v>248</v>
       </c>
       <c r="D197" t="s">
@@ -6071,7 +6085,7 @@
       <c r="B198" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C198" s="11" t="s">
+      <c r="C198" t="s">
         <v>248</v>
       </c>
       <c r="D198" t="s">
@@ -6085,7 +6099,7 @@
       <c r="B199" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C199" s="11" t="s">
+      <c r="C199" t="s">
         <v>248</v>
       </c>
       <c r="D199" t="s">
@@ -6099,7 +6113,7 @@
       <c r="B200" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C200" s="11" t="s">
+      <c r="C200" t="s">
         <v>248</v>
       </c>
       <c r="D200" t="s">
@@ -6113,7 +6127,7 @@
       <c r="B201" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C201" s="11" t="s">
+      <c r="C201" t="s">
         <v>248</v>
       </c>
       <c r="D201" t="s">
@@ -6127,7 +6141,7 @@
       <c r="B202" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C202" s="11" t="s">
+      <c r="C202" t="s">
         <v>248</v>
       </c>
       <c r="D202" t="s">
@@ -6141,7 +6155,7 @@
       <c r="B203" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C203" s="11" t="s">
+      <c r="C203" t="s">
         <v>248</v>
       </c>
       <c r="D203" t="s">
@@ -6155,7 +6169,7 @@
       <c r="B204" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C204" s="11" t="s">
+      <c r="C204" t="s">
         <v>248</v>
       </c>
       <c r="D204" t="s">
@@ -6169,7 +6183,7 @@
       <c r="B205" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C205" s="11" t="s">
+      <c r="C205" t="s">
         <v>248</v>
       </c>
       <c r="D205" t="s">
@@ -6183,7 +6197,7 @@
       <c r="B206" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C206" s="11" t="s">
+      <c r="C206" t="s">
         <v>248</v>
       </c>
       <c r="D206" t="s">
@@ -6197,7 +6211,7 @@
       <c r="B207" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C207" s="11" t="s">
+      <c r="C207" t="s">
         <v>248</v>
       </c>
       <c r="D207" t="s">
@@ -6211,7 +6225,7 @@
       <c r="B208" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C208" s="11" t="s">
+      <c r="C208" t="s">
         <v>248</v>
       </c>
       <c r="D208" t="s">
@@ -6225,7 +6239,7 @@
       <c r="B209" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C209" s="11" t="s">
+      <c r="C209" t="s">
         <v>248</v>
       </c>
       <c r="D209" t="s">
@@ -6239,7 +6253,7 @@
       <c r="B210" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C210" s="11" t="s">
+      <c r="C210" t="s">
         <v>248</v>
       </c>
       <c r="D210" t="s">
@@ -6253,7 +6267,7 @@
       <c r="B211" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C211" s="11" t="s">
+      <c r="C211" t="s">
         <v>248</v>
       </c>
       <c r="D211" t="s">
@@ -6267,7 +6281,7 @@
       <c r="B212" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C212" s="11" t="s">
+      <c r="C212" t="s">
         <v>248</v>
       </c>
       <c r="D212" t="s">
@@ -6281,7 +6295,7 @@
       <c r="B213" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C213" s="11" t="s">
+      <c r="C213" t="s">
         <v>248</v>
       </c>
       <c r="D213" t="s">
@@ -6939,7 +6953,7 @@
       <c r="B260" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C260" s="11" t="s">
+      <c r="C260" t="s">
         <v>187</v>
       </c>
       <c r="D260" t="s">
@@ -7128,7 +7142,7 @@
       <c r="B274" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C274" s="11" t="s">
+      <c r="C274" t="s">
         <v>248</v>
       </c>
       <c r="D274" t="s">
@@ -7142,7 +7156,7 @@
       <c r="B275" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C275" s="11" t="s">
+      <c r="C275" t="s">
         <v>248</v>
       </c>
       <c r="D275" t="s">
@@ -7156,7 +7170,7 @@
       <c r="B276" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C276" s="11" t="s">
+      <c r="C276" t="s">
         <v>248</v>
       </c>
       <c r="D276" t="s">
@@ -7170,7 +7184,7 @@
       <c r="B277" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C277" s="11" t="s">
+      <c r="C277" t="s">
         <v>259</v>
       </c>
       <c r="D277" t="s">
@@ -7184,7 +7198,7 @@
       <c r="B278" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C278" s="11" t="s">
+      <c r="C278" t="s">
         <v>260</v>
       </c>
       <c r="D278" t="s">
@@ -7198,11 +7212,67 @@
       <c r="B279" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C279" s="11" t="s">
+      <c r="C279" t="s">
         <v>261</v>
       </c>
       <c r="D279" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A280" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B280" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="C280" t="s">
+        <v>263</v>
+      </c>
+      <c r="D280" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A281" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B281" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="C281" t="s">
+        <v>264</v>
+      </c>
+      <c r="D281" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A282" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B282" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="C282" t="s">
+        <v>265</v>
+      </c>
+      <c r="D282" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A283" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B283" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="C283" t="s">
+        <v>266</v>
+      </c>
+      <c r="D283" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>